<commit_message>
Fix bugs of locally merging
</commit_message>
<xml_diff>
--- a/Home_WritingCat/repository/Structured Collocations Example.xlsx
+++ b/Home_WritingCat/repository/Structured Collocations Example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Code\writingHelper\Home_WritingCat\repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD71E48-0909-493C-A7B4-EB63503CCC95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27234326-6008-4ECE-9DB5-08194E8D370A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{489BDAD6-CB6B-4906-BCD2-586DEE0C84BC}"/>
   </bookViews>
@@ -1569,15 +1569,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C852DF-D2A1-435D-B58E-339D156780E5}">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B63" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="59.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -3247,6 +3247,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations xWindow="110" yWindow="267" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{DE23D013-E59D-4AAD-AB74-511E3384433A}">
+      <formula1>"culture,duty,efficient,environment,finance,fun,healthy,right,skill,safety,work,life,link"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix Bugs of img
</commit_message>
<xml_diff>
--- a/Home_WritingCat/repository/Structured Collocations Example.xlsx
+++ b/Home_WritingCat/repository/Structured Collocations Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Code\writingHelper\Home_WritingCat\repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27234326-6008-4ECE-9DB5-08194E8D370A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6714E26C-9F52-4F31-ADB0-F7D705ACD157}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{489BDAD6-CB6B-4906-BCD2-586DEE0C84BC}"/>
   </bookViews>
@@ -1567,10 +1567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C852DF-D2A1-435D-B58E-339D156780E5}">
-  <dimension ref="A1:H96"/>
+  <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2544,13 +2544,13 @@
         <v>148</v>
       </c>
       <c r="C56" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D56" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="E56" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2561,13 +2561,13 @@
         <v>148</v>
       </c>
       <c r="C57" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D57" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E57" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2578,13 +2578,13 @@
         <v>148</v>
       </c>
       <c r="C58" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D58" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E58" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2595,13 +2595,13 @@
         <v>148</v>
       </c>
       <c r="C59" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D59" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E59" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2612,13 +2612,13 @@
         <v>148</v>
       </c>
       <c r="C60" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D60" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E60" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2626,16 +2626,16 @@
         <v>0</v>
       </c>
       <c r="B61" t="s">
-        <v>148</v>
+        <v>185</v>
       </c>
       <c r="C61" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="D61" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E61" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2646,13 +2646,13 @@
         <v>185</v>
       </c>
       <c r="C62" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D62" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E62" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2663,13 +2663,13 @@
         <v>185</v>
       </c>
       <c r="C63" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D63" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E63" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2680,13 +2680,13 @@
         <v>185</v>
       </c>
       <c r="C64" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D64" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E64" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2697,13 +2697,13 @@
         <v>185</v>
       </c>
       <c r="C65" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D65" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="E65" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2714,13 +2714,13 @@
         <v>185</v>
       </c>
       <c r="C66" t="s">
-        <v>198</v>
+        <v>95</v>
       </c>
       <c r="D66" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E66" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2731,13 +2731,13 @@
         <v>185</v>
       </c>
       <c r="C67" t="s">
-        <v>95</v>
+        <v>204</v>
       </c>
       <c r="D67" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E67" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2748,13 +2748,13 @@
         <v>185</v>
       </c>
       <c r="C68" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D68" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="E68" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2765,13 +2765,13 @@
         <v>185</v>
       </c>
       <c r="C69" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D69" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E69" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2782,13 +2782,13 @@
         <v>185</v>
       </c>
       <c r="C70" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D70" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="E70" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2799,13 +2799,13 @@
         <v>185</v>
       </c>
       <c r="C71" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D71" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E71" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2813,16 +2813,16 @@
         <v>0</v>
       </c>
       <c r="B72" t="s">
-        <v>185</v>
+        <v>218</v>
       </c>
       <c r="C72" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D72" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="E72" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2830,16 +2830,16 @@
         <v>0</v>
       </c>
       <c r="B73" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C73" t="s">
-        <v>219</v>
+        <v>56</v>
       </c>
       <c r="D73" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E73" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2847,16 +2847,16 @@
         <v>0</v>
       </c>
       <c r="B74" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C74" t="s">
-        <v>56</v>
+        <v>226</v>
       </c>
       <c r="D74" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="E74" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2864,16 +2864,16 @@
         <v>0</v>
       </c>
       <c r="B75" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="C75" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D75" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="E75" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2881,16 +2881,16 @@
         <v>0</v>
       </c>
       <c r="B76" t="s">
-        <v>229</v>
+        <v>6</v>
       </c>
       <c r="C76" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
       <c r="D76" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="E76" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2898,16 +2898,16 @@
         <v>0</v>
       </c>
       <c r="B77" t="s">
-        <v>6</v>
+        <v>247</v>
       </c>
       <c r="C77" t="s">
         <v>244</v>
       </c>
       <c r="D77" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E77" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2915,16 +2915,16 @@
         <v>0</v>
       </c>
       <c r="B78" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="C78" t="s">
         <v>244</v>
       </c>
       <c r="D78" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="E78" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2932,16 +2932,16 @@
         <v>0</v>
       </c>
       <c r="B79" t="s">
-        <v>229</v>
+        <v>104</v>
       </c>
       <c r="C79" t="s">
         <v>244</v>
       </c>
       <c r="D79" t="s">
-        <v>248</v>
+        <v>127</v>
       </c>
       <c r="E79" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2949,16 +2949,16 @@
         <v>0</v>
       </c>
       <c r="B80" t="s">
-        <v>104</v>
+        <v>4</v>
       </c>
       <c r="C80" t="s">
-        <v>244</v>
+        <v>269</v>
       </c>
       <c r="D80" t="s">
-        <v>127</v>
+        <v>279</v>
       </c>
       <c r="E80" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -2972,10 +2972,10 @@
         <v>269</v>
       </c>
       <c r="D81" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E81" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -2983,16 +2983,16 @@
         <v>0</v>
       </c>
       <c r="B82" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C82" t="s">
-        <v>269</v>
+        <v>247</v>
       </c>
       <c r="D82" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="E82" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -3000,16 +3000,16 @@
         <v>0</v>
       </c>
       <c r="B83" t="s">
-        <v>14</v>
+        <v>247</v>
       </c>
       <c r="C83" t="s">
-        <v>247</v>
+        <v>270</v>
       </c>
       <c r="D83" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E83" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -3023,10 +3023,10 @@
         <v>270</v>
       </c>
       <c r="D84" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E84" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -3040,10 +3040,10 @@
         <v>270</v>
       </c>
       <c r="D85" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="E85" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -3057,10 +3057,10 @@
         <v>270</v>
       </c>
       <c r="D86" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E86" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -3068,16 +3068,16 @@
         <v>0</v>
       </c>
       <c r="B87" t="s">
-        <v>247</v>
+        <v>6</v>
       </c>
       <c r="C87" t="s">
         <v>270</v>
       </c>
       <c r="D87" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E87" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3085,16 +3085,16 @@
         <v>0</v>
       </c>
       <c r="B88" t="s">
-        <v>6</v>
+        <v>247</v>
       </c>
       <c r="C88" t="s">
         <v>270</v>
       </c>
       <c r="D88" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E88" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3108,10 +3108,13 @@
         <v>270</v>
       </c>
       <c r="D89" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="E89" t="s">
-        <v>260</v>
+        <v>262</v>
+      </c>
+      <c r="G89" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -3125,13 +3128,13 @@
         <v>270</v>
       </c>
       <c r="D90" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E90" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G90" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -3148,10 +3151,10 @@
         <v>275</v>
       </c>
       <c r="E91" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="G91" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -3168,10 +3171,10 @@
         <v>275</v>
       </c>
       <c r="E92" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G92" t="s">
-        <v>277</v>
+        <v>288</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3179,19 +3182,16 @@
         <v>0</v>
       </c>
       <c r="B93" t="s">
-        <v>247</v>
+        <v>6</v>
       </c>
       <c r="C93" t="s">
         <v>270</v>
       </c>
       <c r="D93" t="s">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="E93" t="s">
-        <v>265</v>
-      </c>
-      <c r="G93" t="s">
-        <v>288</v>
+        <v>266</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -3199,16 +3199,16 @@
         <v>0</v>
       </c>
       <c r="B94" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C94" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D94" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E94" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -3219,36 +3219,19 @@
         <v>14</v>
       </c>
       <c r="C95" t="s">
-        <v>271</v>
+        <v>31</v>
       </c>
       <c r="D95" t="s">
-        <v>290</v>
+        <v>267</v>
       </c>
       <c r="E95" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>0</v>
-      </c>
-      <c r="B96" t="s">
-        <v>14</v>
-      </c>
-      <c r="C96" t="s">
-        <v>31</v>
-      </c>
-      <c r="D96" t="s">
-        <v>267</v>
-      </c>
-      <c r="E96" t="s">
         <v>268</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations xWindow="110" yWindow="267" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{DE23D013-E59D-4AAD-AB74-511E3384433A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B55 B56:B1048576" xr:uid="{DE23D013-E59D-4AAD-AB74-511E3384433A}">
       <formula1>"culture,duty,efficient,environment,finance,fun,healthy,right,skill,safety,work,life,link"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3259,10 +3242,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4859F9C6-9D37-4857-802C-84CC351AC29C}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3317,8 +3300,30 @@
         <v>272</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3" t="s">
+        <v>169</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{DE23D013-E59D-4AAD-AB74-511E3384433A}">
+      <formula1>"culture,duty,efficient,environment,finance,fun,healthy,right,skill,safety,work,life,link"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>